<commit_message>
update code after merge
</commit_message>
<xml_diff>
--- a/src/test/resources/Data.xlsx
+++ b/src/test/resources/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JAVA project\Testing05_Nhom2\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351B4277-95D1-4F9F-96E9-62D58706CD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CA56FB-BC8B-4ECD-AA56-79A8D439778B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5568" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{0C03C9B1-B188-402C-8949-FC84BB5B4FF3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C03C9B1-B188-402C-8949-FC84BB5B4FF3}"/>
   </bookViews>
   <sheets>
     <sheet name="data1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Email</t>
   </si>
   <si>
     <t>Password</t>
-  </si>
-  <si>
-    <t>STT</t>
   </si>
   <si>
     <t>blue299</t>
@@ -50,7 +47,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -59,7 +56,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -111,9 +108,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -151,7 +148,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -257,7 +254,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -399,7 +396,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -407,48 +404,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E40D1DE-244C-42B8-97ED-ADAED0432D20}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
-    <col min="3" max="3" width="26.21875" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="26.09765625" customWidth="1"/>
+    <col min="2" max="2" width="26.19921875" customWidth="1"/>
+    <col min="3" max="3" width="17.59765625" customWidth="1"/>
+    <col min="4" max="4" width="17.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+      <c r="B2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{39DF870C-DC42-4E1B-AAF5-797254371C9B}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{39DF870C-DC42-4E1B-AAF5-797254371C9B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>